<commit_message>
remove some redundant codes
</commit_message>
<xml_diff>
--- a/princess_connect_support/bin/Release/戰隊戰.xlsx
+++ b/princess_connect_support/bin/Release/戰隊戰.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="110">
   <si>
     <t>亞里莎</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -359,6 +359,102 @@
   </si>
   <si>
     <t>上下兩隻犬傷害差好多?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>龍二</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>日和</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>原一三隊互換與捨棄月月借四星犬好像不一定比較好?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>純(借五)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>深月</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>真步</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>栞</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>布丁</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>望</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>月月(借四)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>放栞 15秒犬會死 5秒366647</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>原隊伍 4秒 298330</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>栞</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>惠理子</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>純</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>望</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>爆弓</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>亞里莎</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>深月</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>優衣</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>純(借五)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>鹿二</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>月月(借四)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>純(借四)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -709,10 +805,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N97"/>
+  <dimension ref="A1:N144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="E89" sqref="E89"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="G124" sqref="G124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1993,10 +2089,571 @@
         <v>79</v>
       </c>
     </row>
-    <row r="97" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G97" t="s">
         <v>80</v>
       </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99" s="1">
+        <v>43371</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>18</v>
+      </c>
+      <c r="B100" t="s">
+        <v>17</v>
+      </c>
+      <c r="C100" t="s">
+        <v>29</v>
+      </c>
+      <c r="D100" t="s">
+        <v>87</v>
+      </c>
+      <c r="E100" t="s">
+        <v>14</v>
+      </c>
+      <c r="F100">
+        <v>255129</v>
+      </c>
+      <c r="G100" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>81</v>
+      </c>
+      <c r="B101">
+        <v>81</v>
+      </c>
+      <c r="C101">
+        <v>81</v>
+      </c>
+      <c r="D101">
+        <v>81</v>
+      </c>
+      <c r="E101">
+        <v>78</v>
+      </c>
+      <c r="F101" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>33890</v>
+      </c>
+      <c r="B102">
+        <v>67486</v>
+      </c>
+      <c r="C102">
+        <v>81793</v>
+      </c>
+      <c r="D102">
+        <v>60450</v>
+      </c>
+      <c r="E102">
+        <v>11510</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>27</v>
+      </c>
+      <c r="B104" t="s">
+        <v>8</v>
+      </c>
+      <c r="C104" t="s">
+        <v>12</v>
+      </c>
+      <c r="D104" t="s">
+        <v>3</v>
+      </c>
+      <c r="E104" t="s">
+        <v>37</v>
+      </c>
+      <c r="F104">
+        <v>464926</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>81</v>
+      </c>
+      <c r="B105">
+        <v>81</v>
+      </c>
+      <c r="C105">
+        <v>81</v>
+      </c>
+      <c r="D105">
+        <v>81</v>
+      </c>
+      <c r="E105">
+        <v>81</v>
+      </c>
+      <c r="F105" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>132869</v>
+      </c>
+      <c r="B106">
+        <v>43984</v>
+      </c>
+      <c r="C106">
+        <v>89846</v>
+      </c>
+      <c r="D106">
+        <v>180740</v>
+      </c>
+      <c r="E106">
+        <v>17487</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>16</v>
+      </c>
+      <c r="B108" t="s">
+        <v>28</v>
+      </c>
+      <c r="C108" t="s">
+        <v>1</v>
+      </c>
+      <c r="D108" t="s">
+        <v>82</v>
+      </c>
+      <c r="E108" t="s">
+        <v>9</v>
+      </c>
+      <c r="F108">
+        <v>339827</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A109">
+        <v>81</v>
+      </c>
+      <c r="B109">
+        <v>81</v>
+      </c>
+      <c r="C109">
+        <v>81</v>
+      </c>
+      <c r="D109">
+        <v>81</v>
+      </c>
+      <c r="E109">
+        <v>81</v>
+      </c>
+      <c r="F109" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A110">
+        <v>89727</v>
+      </c>
+      <c r="B110">
+        <v>68660</v>
+      </c>
+      <c r="C110">
+        <v>31827</v>
+      </c>
+      <c r="D110">
+        <v>137266</v>
+      </c>
+      <c r="E110">
+        <v>12347</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F111">
+        <f>SUM(F100:F109)</f>
+        <v>1059882</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A114" s="1">
+        <v>43372</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>18</v>
+      </c>
+      <c r="B115" t="s">
+        <v>92</v>
+      </c>
+      <c r="C115" t="s">
+        <v>95</v>
+      </c>
+      <c r="D115" t="s">
+        <v>94</v>
+      </c>
+      <c r="E115" t="s">
+        <v>93</v>
+      </c>
+      <c r="F115">
+        <v>220766</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>81</v>
+      </c>
+      <c r="B116">
+        <v>81</v>
+      </c>
+      <c r="C116">
+        <v>81</v>
+      </c>
+      <c r="D116">
+        <v>81</v>
+      </c>
+      <c r="E116">
+        <v>78</v>
+      </c>
+      <c r="F116" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>35703</v>
+      </c>
+      <c r="B117">
+        <v>90789</v>
+      </c>
+      <c r="C117">
+        <v>67119</v>
+      </c>
+      <c r="D117">
+        <v>14122</v>
+      </c>
+      <c r="E117">
+        <v>13033</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>91</v>
+      </c>
+      <c r="B119" t="s">
+        <v>90</v>
+      </c>
+      <c r="C119" t="s">
+        <v>8</v>
+      </c>
+      <c r="D119" t="s">
+        <v>3</v>
+      </c>
+      <c r="E119" t="s">
+        <v>89</v>
+      </c>
+      <c r="F119">
+        <v>209698</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>81</v>
+      </c>
+      <c r="B120">
+        <v>81</v>
+      </c>
+      <c r="C120">
+        <v>81</v>
+      </c>
+      <c r="D120">
+        <v>81</v>
+      </c>
+      <c r="E120">
+        <v>81</v>
+      </c>
+      <c r="F120" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>11417</v>
+      </c>
+      <c r="B121">
+        <v>29622</v>
+      </c>
+      <c r="C121">
+        <v>35400</v>
+      </c>
+      <c r="D121">
+        <v>120614</v>
+      </c>
+      <c r="E121">
+        <v>12645</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>16</v>
+      </c>
+      <c r="B123" t="s">
+        <v>28</v>
+      </c>
+      <c r="C123" t="s">
+        <v>1</v>
+      </c>
+      <c r="D123" t="s">
+        <v>82</v>
+      </c>
+      <c r="E123" t="s">
+        <v>9</v>
+      </c>
+      <c r="F123">
+        <v>339827</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>81</v>
+      </c>
+      <c r="B124">
+        <v>81</v>
+      </c>
+      <c r="C124">
+        <v>81</v>
+      </c>
+      <c r="D124">
+        <v>81</v>
+      </c>
+      <c r="E124">
+        <v>81</v>
+      </c>
+      <c r="F124" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>89727</v>
+      </c>
+      <c r="B125">
+        <v>68660</v>
+      </c>
+      <c r="C125">
+        <v>31827</v>
+      </c>
+      <c r="D125">
+        <v>200000</v>
+      </c>
+      <c r="E125">
+        <v>12347</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F126">
+        <f>SUM(F115:F124)</f>
+        <v>770291</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A128" s="1"/>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A129" s="1">
+        <v>43373</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>98</v>
+      </c>
+      <c r="B130" t="s">
+        <v>99</v>
+      </c>
+      <c r="C130" t="s">
+        <v>108</v>
+      </c>
+      <c r="D130" t="s">
+        <v>101</v>
+      </c>
+      <c r="E130" t="s">
+        <v>100</v>
+      </c>
+      <c r="F130">
+        <v>305305</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>82</v>
+      </c>
+      <c r="B131">
+        <v>82</v>
+      </c>
+      <c r="C131">
+        <v>78</v>
+      </c>
+      <c r="D131">
+        <v>82</v>
+      </c>
+      <c r="E131">
+        <v>82</v>
+      </c>
+      <c r="F131" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>139313</v>
+      </c>
+      <c r="B132">
+        <v>101079</v>
+      </c>
+      <c r="C132">
+        <v>44387</v>
+      </c>
+      <c r="D132">
+        <v>11033</v>
+      </c>
+      <c r="E132">
+        <v>9493</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>105</v>
+      </c>
+      <c r="B134" t="s">
+        <v>8</v>
+      </c>
+      <c r="C134" t="s">
+        <v>3</v>
+      </c>
+      <c r="D134" t="s">
+        <v>12</v>
+      </c>
+      <c r="E134" t="s">
+        <v>106</v>
+      </c>
+      <c r="F134">
+        <v>303519</v>
+      </c>
+      <c r="G134" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>82</v>
+      </c>
+      <c r="B135">
+        <v>82</v>
+      </c>
+      <c r="C135">
+        <v>82</v>
+      </c>
+      <c r="D135">
+        <v>82</v>
+      </c>
+      <c r="E135">
+        <v>80</v>
+      </c>
+      <c r="F135" t="s">
+        <v>107</v>
+      </c>
+      <c r="G135" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>24206</v>
+      </c>
+      <c r="B136">
+        <v>51506</v>
+      </c>
+      <c r="C136">
+        <v>145790</v>
+      </c>
+      <c r="D136">
+        <v>65251</v>
+      </c>
+      <c r="E136">
+        <v>16766</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>102</v>
+      </c>
+      <c r="B138" t="s">
+        <v>103</v>
+      </c>
+      <c r="C138" t="s">
+        <v>104</v>
+      </c>
+      <c r="D138" t="s">
+        <v>13</v>
+      </c>
+      <c r="E138" t="s">
+        <v>109</v>
+      </c>
+      <c r="F138">
+        <v>226616</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>82</v>
+      </c>
+      <c r="B139">
+        <v>82</v>
+      </c>
+      <c r="C139">
+        <v>82</v>
+      </c>
+      <c r="D139">
+        <v>82</v>
+      </c>
+      <c r="E139">
+        <v>79</v>
+      </c>
+      <c r="F139" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>100794</v>
+      </c>
+      <c r="B140">
+        <v>90952</v>
+      </c>
+      <c r="C140">
+        <v>19049</v>
+      </c>
+      <c r="D140">
+        <v>7973</v>
+      </c>
+      <c r="E140">
+        <v>7848</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F141">
+        <f>SUM(F130:F139)</f>
+        <v>835440</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A144" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>